<commit_message>
fix URI error for version of record
</commit_message>
<xml_diff>
--- a/scripts/infoscience-map.xlsx
+++ b/scripts/infoscience-map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sicot/Devs/dspace_dev/infoscience-map/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4385A311-E0FE-B64A-9197-91C863F1D4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFE052F-DF4B-284F-8E5B-EABB5F5CA38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30000" yWindow="1800" windowWidth="27640" windowHeight="16940" xr2:uid="{C1497B1D-5E77-6240-B8B6-95DADB08CE76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="784">
   <si>
     <t>name</t>
   </si>
@@ -2385,6 +2385,9 @@
   </si>
   <si>
     <t>Book Chapters,Books,Conference Papers,Conference Proceedings,Datasets,Journal Articles,Media,Patents,Posters,Physical objects,Reports,Reviews,Student Projects,Talks,Teaching Material,Theses,Working Papers</t>
+  </si>
+  <si>
+    <t>http://purl.org/coar/version/c_71e4c1898caa6e32 (submitted version or preprint),http://purl.org/coar/version/c_ab4af688f83e57aa (accepted version or accepted manuscript),http://purl.org/coar/version/c_970fb48d4fbd8a85 (published version),http://purl.org/coar/version/c_e19f295774971610 (corrected version) , http://purl.org/coar/version/c_e19f295774971610 (not applicable or unknown)</t>
   </si>
 </sst>
 </file>
@@ -2767,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB157D6-8822-6144-895F-63A11089911B}">
   <dimension ref="A1:Q108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="H84" workbookViewId="0">
+      <selection activeCell="N116" sqref="N116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7765,7 +7768,7 @@
         <v>587</v>
       </c>
       <c r="N108" t="s">
-        <v>588</v>
+        <v>783</v>
       </c>
       <c r="O108" t="s">
         <v>27</v>

</xml_diff>